<commit_message>
Commit on 14 sept 2022
</commit_message>
<xml_diff>
--- a/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
+++ b/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AllMastersTestDataInfo" sheetId="7" r:id="rId1"/>
     <sheet name="AllMasterInstructions" sheetId="6" r:id="rId2"/>
     <sheet name="AssetAutoMasterTestData" sheetId="4" r:id="rId3"/>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId4"/>
-    <sheet name="ReportMasterTestData" sheetId="8" r:id="rId5"/>
-    <sheet name="SubProductMasterRetail" sheetId="9" r:id="rId6"/>
-    <sheet name="UnderWriterOffSetTestData" sheetId="11" r:id="rId7"/>
+    <sheet name="SubProductMasterRetail" sheetId="9" r:id="rId5"/>
+    <sheet name="UnderWriterOffSetTestData" sheetId="11" r:id="rId6"/>
+    <sheet name="ReportMasterTestData1" sheetId="12" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="409">
   <si>
     <t>Reference ID</t>
   </si>
@@ -426,204 +427,27 @@
     <t>ASSEt</t>
   </si>
   <si>
-    <t>AT-RA-001</t>
-  </si>
-  <si>
-    <t>AT-RA-002</t>
-  </si>
-  <si>
-    <t>AT-RA-003</t>
-  </si>
-  <si>
-    <t>AT-RA-004</t>
-  </si>
-  <si>
     <t>AT-RA-005</t>
   </si>
   <si>
-    <t>AT-RA-006</t>
-  </si>
-  <si>
-    <t>AT-RA-007</t>
-  </si>
-  <si>
-    <t>AT-RA-008</t>
-  </si>
-  <si>
-    <t>AT-RA-009</t>
-  </si>
-  <si>
     <t>AT-RA-010</t>
   </si>
   <si>
-    <t>AT-RA-011</t>
-  </si>
-  <si>
-    <t>AT-RA-012</t>
-  </si>
-  <si>
-    <t>AT-RA-013</t>
-  </si>
-  <si>
-    <t>AT-RA-014</t>
-  </si>
-  <si>
-    <t>AT-RA-015</t>
-  </si>
-  <si>
     <t>AT-RA-016</t>
   </si>
   <si>
-    <t>AT-RA-017</t>
-  </si>
-  <si>
-    <t>AT-RA-018</t>
-  </si>
-  <si>
-    <t>AT-RA-019</t>
-  </si>
-  <si>
-    <t>AT-RA-020</t>
-  </si>
-  <si>
-    <t>AT-RA-021</t>
-  </si>
-  <si>
-    <t>AT-RA-022</t>
-  </si>
-  <si>
-    <t>AT-RA-023</t>
-  </si>
-  <si>
-    <t>AT-RA-024</t>
-  </si>
-  <si>
-    <t>AT-RA-025</t>
-  </si>
-  <si>
-    <t>AT-RA-026</t>
-  </si>
-  <si>
-    <t>AT-RA-027</t>
-  </si>
-  <si>
-    <t>AT-RA-028</t>
-  </si>
-  <si>
-    <t>AT-RA-029</t>
-  </si>
-  <si>
-    <t>AT-RA-030</t>
-  </si>
-  <si>
-    <t>AT-RA-031</t>
-  </si>
-  <si>
-    <t>AT-RA-032</t>
-  </si>
-  <si>
-    <t>AT-RA-033</t>
-  </si>
-  <si>
-    <t>AT-RA-034</t>
-  </si>
-  <si>
-    <t>AT-RA-035</t>
-  </si>
-  <si>
-    <t>AT-RA-036</t>
-  </si>
-  <si>
-    <t>AT-RA-037</t>
-  </si>
-  <si>
-    <t>AT-RA-038</t>
-  </si>
-  <si>
-    <t>AT-RA-039</t>
-  </si>
-  <si>
-    <t>AT-RA-040</t>
-  </si>
-  <si>
-    <t>AT-RA-041</t>
-  </si>
-  <si>
-    <t>AT-RA-042</t>
-  </si>
-  <si>
     <t>AT-RA-001_D1</t>
   </si>
   <si>
     <t>AT-RA-001_D2</t>
   </si>
   <si>
-    <t>ReportName</t>
-  </si>
-  <si>
-    <t>ReportName2</t>
-  </si>
-  <si>
-    <t>ReportName3</t>
-  </si>
-  <si>
-    <t>ReportDescription</t>
-  </si>
-  <si>
-    <t>ReportType</t>
-  </si>
-  <si>
-    <t>ReportUrl</t>
-  </si>
-  <si>
-    <t>ReportCategory</t>
-  </si>
-  <si>
-    <t>SearchReportMaster</t>
-  </si>
-  <si>
-    <t>EnterRemark</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>CRY</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
-  </si>
-  <si>
-    <t>https://cliqz.com/en/report-url</t>
-  </si>
-  <si>
-    <t>MST_REPORT</t>
-  </si>
-  <si>
     <t>AT-RA-007_D1</t>
   </si>
   <si>
     <t>AT-RA-001_D3</t>
   </si>
   <si>
-    <t>AT-RA-001_D4</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D5</t>
-  </si>
-  <si>
     <t>AT-RA-001_D6</t>
   </si>
   <si>
@@ -654,102 +478,12 @@
     <t>AT-RA-001_D16</t>
   </si>
   <si>
-    <t>AT-RA-001_D17</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D18</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D19</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D20</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D21</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D22</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D23</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D24</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D25</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D26</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D27</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D28</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D29</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D30</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D31</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D32</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D33</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D34</t>
-  </si>
-  <si>
-    <t>AT-RA-001_D35</t>
-  </si>
-  <si>
     <t>AT-RA-007_D2</t>
   </si>
   <si>
     <t>AT-RA-007_D3</t>
   </si>
   <si>
-    <t>Company1</t>
-  </si>
-  <si>
-    <t>Company2</t>
-  </si>
-  <si>
-    <t>Credit1</t>
-  </si>
-  <si>
-    <t>Credit2</t>
-  </si>
-  <si>
-    <t>Report1</t>
-  </si>
-  <si>
-    <t>Report2</t>
-  </si>
-  <si>
-    <t>BIR</t>
-  </si>
-  <si>
-    <t>OBI</t>
-  </si>
-  <si>
-    <t>REPORT</t>
-  </si>
-  <si>
-    <t>MISR</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Maker1</t>
   </si>
   <si>
@@ -1485,22 +1219,52 @@
     <t>AT_UOC_T005_D4</t>
   </si>
   <si>
-    <t>5356</t>
-  </si>
-  <si>
-    <t>5357</t>
-  </si>
-  <si>
-    <t>5358</t>
-  </si>
-  <si>
-    <t>5359</t>
-  </si>
-  <si>
-    <t>5360</t>
-  </si>
-  <si>
-    <t>5365</t>
+    <t>CharecterInputs</t>
+  </si>
+  <si>
+    <t>abcABC12</t>
+  </si>
+  <si>
+    <t>SpecialCharecterValidationMessage</t>
+  </si>
+  <si>
+    <t>NumericInput</t>
+  </si>
+  <si>
+    <t>TemplateIDInput</t>
+  </si>
+  <si>
+    <t>isMandatory</t>
+  </si>
+  <si>
+    <t>defaultSelectValue</t>
+  </si>
+  <si>
+    <t>mandatoryFieldValidationMessage</t>
+  </si>
+  <si>
+    <t>Alphanumeric characters allowed</t>
+  </si>
+  <si>
+    <t>Required field</t>
+  </si>
+  <si>
+    <t>AT-RA-005_D1</t>
+  </si>
+  <si>
+    <t>AT-RA-010_D1</t>
+  </si>
+  <si>
+    <t>AT-RA-016_D1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Language Id</t>
   </si>
 </sst>
 </file>
@@ -1536,13 +1300,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1609,8 +1366,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1671,8 +1435,14 @@
         <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1769,30 +1539,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1867,27 +1646,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1905,49 +1666,62 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="10" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="10" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="10">
-    <cellStyle name="Excel Built-in Hyperlink" xfId="5"/>
-    <cellStyle name="Excel Built-in Normal" xfId="2"/>
-    <cellStyle name="Heading" xfId="6"/>
-    <cellStyle name="Heading1" xfId="7"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4"/>
+  <cellStyles count="9">
+    <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Heading" xfId="5"/>
+    <cellStyle name="Heading1" xfId="6"/>
+    <cellStyle name="Hyperlink 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Result" xfId="8"/>
-    <cellStyle name="Result2" xfId="9"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Result" xfId="7"/>
+    <cellStyle name="Result2" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2255,12 +2029,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" hidden="true" width="21.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="11" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="4.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="11" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.140625" hidden="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2306,7 +2080,7 @@
       <c r="F2" s="17">
         <v>44837</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="36">
         <v>1</v>
       </c>
     </row>
@@ -2329,7 +2103,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>152</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2338,9 +2112,9 @@
         <v>ReportMaster_TD-10-10-2022</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" s="48">
+        <v>153</v>
+      </c>
+      <c r="F4" s="38">
         <v>44844</v>
       </c>
     </row>
@@ -2350,7 +2124,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="47"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
@@ -2358,7 +2132,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="47"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
@@ -2366,7 +2140,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="47"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2"/>
@@ -2374,7 +2148,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="16"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="47"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
@@ -2382,7 +2156,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="47"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
@@ -2390,7 +2164,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="47"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
@@ -2398,7 +2172,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="47"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
@@ -2406,7 +2180,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="47"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
@@ -2414,7 +2188,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="16"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="47"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
@@ -2422,7 +2196,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="47"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
@@ -2430,7 +2204,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="47"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
@@ -2438,7 +2212,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="16"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="47"/>
+      <c r="F16" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2518,36 +2292,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="31" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="18" width="20.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="18" width="12.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="18" width="7.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="18" width="17.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="18" width="20.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="18" width="20.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="18" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="18" width="14.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="18" width="16.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="18" width="21.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="18" width="25.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="18" width="21.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="18" width="24.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="18" width="11.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="18" width="22.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="18" width="10.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="18" width="14.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="18" width="26.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="18" width="17.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="18" width="10.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="18" width="16.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="18" width="24.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="18" width="24.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="18" width="8.5703125" collapsed="true"/>
-    <col min="30" max="16384" style="18" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="21.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="24.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="26" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="16.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="24.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="8.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="16384" width="9.140625" style="18" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="16" customFormat="1">
@@ -2742,10 +2516,10 @@
         <v>77</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>438</v>
+        <v>349</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>441</v>
+        <v>352</v>
       </c>
       <c r="H4" s="22" t="s">
         <v>28</v>
@@ -2782,7 +2556,7 @@
         <v>118</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>442</v>
+        <v>353</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>31</v>
@@ -2952,7 +2726,7 @@
         <v>77</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>439</v>
+        <v>350</v>
       </c>
       <c r="L9" s="21" t="s">
         <v>76</v>
@@ -2998,7 +2772,7 @@
         <v>74</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>440</v>
+        <v>351</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>35</v>
@@ -3515,7 +3289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3531,7 +3305,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>56</v>
@@ -3542,7 +3316,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>238</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>58</v>
@@ -3553,7 +3327,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -3564,7 +3338,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>240</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
@@ -3579,1119 +3353,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="5" max="7" style="10" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="10" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" style="19" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="10" width="39.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="19" width="16.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="13" max="13" style="10" width="13.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="13" customFormat="1">
-      <c r="A1" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75">
-      <c r="A2" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="38"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75">
-      <c r="A4" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="30">
-        <v>908</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" s="30">
-        <v>910</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="30">
-        <v>911</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="K9" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="L9" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="L10" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75">
-      <c r="A12" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75">
-      <c r="A13" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75">
-      <c r="A14" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="C14" s="30">
-        <v>908</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75">
-      <c r="A15" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="C15" s="30">
-        <v>910</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75">
-      <c r="A16" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" s="30">
-        <v>911</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75">
-      <c r="A17" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75">
-      <c r="A18" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75">
-      <c r="A19" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
-      <c r="A21" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C21" s="30">
-        <v>908</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75">
-      <c r="A22" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="C22" s="30">
-        <v>910</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="C23" s="30">
-        <v>911</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75">
-      <c r="A24" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="2"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75">
-      <c r="A28" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C28" s="30">
-        <v>908</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="1:14" ht="15.75">
-      <c r="A29" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="C29" s="30">
-        <v>910</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="1:14" ht="15.75">
-      <c r="A30" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C30" s="30">
-        <v>911</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="2"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75">
-      <c r="A31" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="2"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75">
-      <c r="A32" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="1:14" ht="15.75">
-      <c r="A33" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75">
-      <c r="A34" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="C34" s="30">
-        <v>908</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75">
-      <c r="A35" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="C35" s="30">
-        <v>910</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75">
-      <c r="A36" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="30">
-        <v>911</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75">
-      <c r="A37" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75">
-      <c r="A38" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75">
-      <c r="A39" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="42"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="1:14" ht="15.75">
-      <c r="A40" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="2"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75">
-      <c r="A41" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="30">
-        <v>908</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75">
-      <c r="A42" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C42" s="30">
-        <v>910</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="2"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75">
-      <c r="A43" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="30">
-        <v>911</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="2"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75">
-      <c r="A44" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="2"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75">
-      <c r="A45" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.75">
-      <c r="A46" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="2"/>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
-      <formula1>"ART,CRY,BIR,GRIDB,OBI"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
-      <formula1>"REPORT,TEMPLATE,MISR"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="J9" r:id="rId1"/>
-    <hyperlink ref="J10" r:id="rId2"/>
-    <hyperlink ref="J11" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFC41"/>
   <sheetViews>
@@ -4702,563 +3363,563 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" style="53" width="24.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="62" max="62" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="63" max="63" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="64" max="64" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="66" max="66" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="72" max="72" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="73" max="73" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="75" max="75" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="76" max="76" customWidth="true" width="31.5703125" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="81" max="81" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="89" max="89" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" width="40.7109375" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="98" max="98" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="100" max="100" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="1" max="1" width="24.28515625" style="43" collapsed="1"/>
+    <col min="13" max="13" width="28" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="31.5703125" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="89" max="89" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="29" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="24.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104 16383:16383" s="57" customFormat="1">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:104 16383:16383" s="47" customFormat="1">
+      <c r="A1" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="O1" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="P1" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q1" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="R1" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="S1" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="U1" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="V1" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="W1" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="X1" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z1" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA1" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB1" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC1" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD1" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG1" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH1" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI1" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ1" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="AK1" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="AL1" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM1" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN1" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="AO1" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="AP1" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="AQ1" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="AR1" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="AS1" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT1" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="AU1" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="AV1" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="AW1" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="AX1" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY1" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ1" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="BA1" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="BB1" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC1" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="BD1" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="BE1" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="BF1" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="BG1" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="BH1" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="BI1" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BJ1" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="BK1" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="BL1" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="BM1" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="BN1" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="BO1" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="BP1" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="BQ1" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="BR1" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="BS1" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="BT1" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="BU1" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="BV1" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="BW1" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="BX1" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY1" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="BZ1" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="CA1" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="CB1" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="CC1" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="CD1" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="CE1" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="CF1" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="CG1" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="CH1" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="CI1" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="CJ1" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="CK1" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="CL1" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="CM1" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="CN1" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO1" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="CP1" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="CQ1" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="CR1" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="CS1" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="CT1" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="CU1" s="47" t="s">
         <v>268</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="CV1" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="CW1" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="CX1" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="CY1" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="CZ1" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="O1" s="57" t="s">
+    </row>
+    <row r="2" spans="1:104 16383:16383">
+      <c r="A2" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="32"/>
+      <c r="E2" t="s">
         <v>274</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="F2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" t="s">
+        <v>331</v>
+      </c>
+      <c r="H2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" t="s">
+        <v>283</v>
+      </c>
+      <c r="K2" t="s">
+        <v>284</v>
+      </c>
+      <c r="L2" t="s">
+        <v>287</v>
+      </c>
+      <c r="M2" t="s">
+        <v>289</v>
+      </c>
+      <c r="N2" t="s">
+        <v>291</v>
+      </c>
+      <c r="O2" t="s">
+        <v>293</v>
+      </c>
+      <c r="P2" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>288</v>
+      </c>
+      <c r="R2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T2" t="s">
+        <v>296</v>
+      </c>
+      <c r="U2" t="s">
+        <v>298</v>
+      </c>
+      <c r="V2" t="s">
+        <v>322</v>
+      </c>
+      <c r="W2" t="s">
+        <v>326</v>
+      </c>
+      <c r="XFC2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:104 16383:16383">
+      <c r="A3" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="32"/>
+      <c r="E3" t="s">
         <v>275</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="F3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H3" t="s">
+        <v>338</v>
+      </c>
+      <c r="I3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K3" t="s">
+        <v>285</v>
+      </c>
+      <c r="L3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M3" t="s">
+        <v>290</v>
+      </c>
+      <c r="N3" t="s">
+        <v>292</v>
+      </c>
+      <c r="O3" t="s">
+        <v>294</v>
+      </c>
+      <c r="P3" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>287</v>
+      </c>
+      <c r="R3" t="s">
+        <v>288</v>
+      </c>
+      <c r="S3" t="s">
+        <v>288</v>
+      </c>
+      <c r="T3" t="s">
+        <v>297</v>
+      </c>
+      <c r="U3" t="s">
+        <v>299</v>
+      </c>
+      <c r="V3" t="s">
+        <v>323</v>
+      </c>
+      <c r="W3" t="s">
+        <v>327</v>
+      </c>
+      <c r="XFC3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:104 16383:16383">
+      <c r="A4" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" t="s">
         <v>276</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="F4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G4" t="s">
+        <v>333</v>
+      </c>
+      <c r="H4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" t="s">
+        <v>282</v>
+      </c>
+      <c r="J4" t="s">
+        <v>283</v>
+      </c>
+      <c r="K4" t="s">
+        <v>286</v>
+      </c>
+      <c r="L4" t="s">
+        <v>287</v>
+      </c>
+      <c r="M4" t="s">
+        <v>289</v>
+      </c>
+      <c r="N4" t="s">
+        <v>291</v>
+      </c>
+      <c r="O4" t="s">
+        <v>295</v>
+      </c>
+      <c r="P4" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>287</v>
+      </c>
+      <c r="R4" t="s">
+        <v>287</v>
+      </c>
+      <c r="S4" t="s">
+        <v>287</v>
+      </c>
+      <c r="T4" t="s">
+        <v>296</v>
+      </c>
+      <c r="U4" t="s">
+        <v>300</v>
+      </c>
+      <c r="V4" t="s">
+        <v>324</v>
+      </c>
+      <c r="W4" t="s">
+        <v>328</v>
+      </c>
+      <c r="XFC4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:104 16383:16383">
+      <c r="A5" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>277</v>
-      </c>
-      <c r="S1" s="57" t="s">
-        <v>278</v>
-      </c>
-      <c r="T1" s="57" t="s">
-        <v>279</v>
-      </c>
-      <c r="U1" s="57" t="s">
-        <v>280</v>
-      </c>
-      <c r="V1" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="W1" s="57" t="s">
-        <v>282</v>
-      </c>
-      <c r="X1" s="57" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y1" s="57" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z1" s="57" t="s">
-        <v>285</v>
-      </c>
-      <c r="AA1" s="57" t="s">
-        <v>286</v>
-      </c>
-      <c r="AB1" s="57" t="s">
-        <v>287</v>
-      </c>
-      <c r="AC1" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD1" s="57" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE1" s="57" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF1" s="57" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG1" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="AH1" s="57" t="s">
-        <v>293</v>
-      </c>
-      <c r="AI1" s="57" t="s">
-        <v>294</v>
-      </c>
-      <c r="AJ1" s="57" t="s">
-        <v>295</v>
-      </c>
-      <c r="AK1" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="AL1" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="AM1" s="57" t="s">
-        <v>298</v>
-      </c>
-      <c r="AN1" s="57" t="s">
-        <v>299</v>
-      </c>
-      <c r="AO1" s="57" t="s">
-        <v>300</v>
-      </c>
-      <c r="AP1" s="57" t="s">
-        <v>301</v>
-      </c>
-      <c r="AQ1" s="57" t="s">
-        <v>302</v>
-      </c>
-      <c r="AR1" s="57" t="s">
-        <v>303</v>
-      </c>
-      <c r="AS1" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT1" s="57" t="s">
-        <v>304</v>
-      </c>
-      <c r="AU1" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="AV1" s="57" t="s">
-        <v>306</v>
-      </c>
-      <c r="AW1" s="57" t="s">
-        <v>307</v>
-      </c>
-      <c r="AX1" s="57" t="s">
-        <v>308</v>
-      </c>
-      <c r="AY1" s="57" t="s">
-        <v>309</v>
-      </c>
-      <c r="AZ1" s="57" t="s">
-        <v>310</v>
-      </c>
-      <c r="BA1" s="57" t="s">
-        <v>311</v>
-      </c>
-      <c r="BB1" s="57" t="s">
-        <v>312</v>
-      </c>
-      <c r="BC1" s="57" t="s">
-        <v>313</v>
-      </c>
-      <c r="BD1" s="57" t="s">
-        <v>314</v>
-      </c>
-      <c r="BE1" s="57" t="s">
-        <v>315</v>
-      </c>
-      <c r="BF1" s="57" t="s">
-        <v>316</v>
-      </c>
-      <c r="BG1" s="57" t="s">
-        <v>317</v>
-      </c>
-      <c r="BH1" s="57" t="s">
-        <v>318</v>
-      </c>
-      <c r="BI1" s="57" t="s">
-        <v>319</v>
-      </c>
-      <c r="BJ1" s="57" t="s">
-        <v>320</v>
-      </c>
-      <c r="BK1" s="57" t="s">
-        <v>321</v>
-      </c>
-      <c r="BL1" s="57" t="s">
-        <v>322</v>
-      </c>
-      <c r="BM1" s="57" t="s">
-        <v>323</v>
-      </c>
-      <c r="BN1" s="57" t="s">
-        <v>324</v>
-      </c>
-      <c r="BO1" s="57" t="s">
-        <v>325</v>
-      </c>
-      <c r="BP1" s="57" t="s">
-        <v>326</v>
-      </c>
-      <c r="BQ1" s="57" t="s">
-        <v>327</v>
-      </c>
-      <c r="BR1" s="57" t="s">
-        <v>328</v>
-      </c>
-      <c r="BS1" s="57" t="s">
-        <v>329</v>
-      </c>
-      <c r="BT1" s="57" t="s">
-        <v>330</v>
-      </c>
-      <c r="BU1" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="BV1" s="57" t="s">
-        <v>332</v>
-      </c>
-      <c r="BW1" s="57" t="s">
-        <v>333</v>
-      </c>
-      <c r="BX1" s="57" t="s">
-        <v>334</v>
-      </c>
-      <c r="BY1" s="57" t="s">
-        <v>335</v>
-      </c>
-      <c r="BZ1" s="57" t="s">
-        <v>336</v>
-      </c>
-      <c r="CA1" s="57" t="s">
-        <v>337</v>
-      </c>
-      <c r="CB1" s="57" t="s">
-        <v>338</v>
-      </c>
-      <c r="CC1" s="57" t="s">
-        <v>339</v>
-      </c>
-      <c r="CD1" s="57" t="s">
-        <v>340</v>
-      </c>
-      <c r="CE1" s="57" t="s">
-        <v>341</v>
-      </c>
-      <c r="CF1" s="57" t="s">
-        <v>342</v>
-      </c>
-      <c r="CG1" s="57" t="s">
-        <v>343</v>
-      </c>
-      <c r="CH1" s="57" t="s">
-        <v>344</v>
-      </c>
-      <c r="CI1" s="57" t="s">
-        <v>345</v>
-      </c>
-      <c r="CJ1" s="57" t="s">
-        <v>346</v>
-      </c>
-      <c r="CK1" s="57" t="s">
-        <v>347</v>
-      </c>
-      <c r="CL1" s="57" t="s">
-        <v>348</v>
-      </c>
-      <c r="CM1" s="57" t="s">
-        <v>349</v>
-      </c>
-      <c r="CN1" s="57" t="s">
-        <v>350</v>
-      </c>
-      <c r="CO1" s="57" t="s">
-        <v>351</v>
-      </c>
-      <c r="CP1" s="57" t="s">
-        <v>352</v>
-      </c>
-      <c r="CQ1" s="57" t="s">
-        <v>353</v>
-      </c>
-      <c r="CR1" s="57" t="s">
-        <v>354</v>
-      </c>
-      <c r="CS1" s="57" t="s">
-        <v>355</v>
-      </c>
-      <c r="CT1" s="57" t="s">
-        <v>356</v>
-      </c>
-      <c r="CU1" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="CV1" s="57" t="s">
-        <v>358</v>
-      </c>
-      <c r="CW1" s="57" t="s">
-        <v>359</v>
-      </c>
-      <c r="CX1" s="57" t="s">
-        <v>360</v>
-      </c>
-      <c r="CY1" s="57" t="s">
-        <v>361</v>
-      </c>
-      <c r="CZ1" s="57" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:104 16383:16383">
-      <c r="A2" s="55" t="s">
-        <v>243</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="35"/>
-      <c r="E2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G2" t="s">
-        <v>420</v>
-      </c>
-      <c r="H2" t="s">
-        <v>426</v>
-      </c>
-      <c r="I2" t="s">
-        <v>371</v>
-      </c>
-      <c r="J2" t="s">
-        <v>372</v>
-      </c>
-      <c r="K2" t="s">
-        <v>373</v>
-      </c>
-      <c r="L2" t="s">
-        <v>376</v>
-      </c>
-      <c r="M2" t="s">
-        <v>378</v>
-      </c>
-      <c r="N2" t="s">
-        <v>380</v>
-      </c>
-      <c r="O2" t="s">
-        <v>382</v>
-      </c>
-      <c r="P2" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>377</v>
-      </c>
-      <c r="R2" t="s">
-        <v>376</v>
-      </c>
-      <c r="S2" t="s">
-        <v>376</v>
-      </c>
-      <c r="T2" t="s">
-        <v>385</v>
-      </c>
-      <c r="U2" t="s">
-        <v>387</v>
-      </c>
-      <c r="V2" t="s">
-        <v>411</v>
-      </c>
-      <c r="W2" t="s">
-        <v>415</v>
-      </c>
-      <c r="XFC2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="3" spans="1:104 16383:16383">
-      <c r="A3" s="50" t="s">
-        <v>243</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>262</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="35"/>
-      <c r="E3" t="s">
-        <v>364</v>
-      </c>
-      <c r="F3" t="s">
-        <v>369</v>
-      </c>
-      <c r="G3" t="s">
-        <v>421</v>
-      </c>
-      <c r="H3" t="s">
-        <v>427</v>
-      </c>
-      <c r="I3" t="s">
-        <v>371</v>
-      </c>
-      <c r="J3" t="s">
-        <v>372</v>
-      </c>
-      <c r="K3" t="s">
-        <v>374</v>
-      </c>
-      <c r="L3" t="s">
-        <v>377</v>
-      </c>
-      <c r="M3" t="s">
-        <v>379</v>
-      </c>
-      <c r="N3" t="s">
-        <v>381</v>
-      </c>
-      <c r="O3" t="s">
-        <v>383</v>
-      </c>
-      <c r="P3" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>376</v>
-      </c>
-      <c r="R3" t="s">
-        <v>377</v>
-      </c>
-      <c r="S3" t="s">
-        <v>377</v>
-      </c>
-      <c r="T3" t="s">
-        <v>386</v>
-      </c>
-      <c r="U3" t="s">
-        <v>388</v>
-      </c>
-      <c r="V3" t="s">
-        <v>412</v>
-      </c>
-      <c r="W3" t="s">
-        <v>416</v>
-      </c>
-      <c r="XFC3" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="4" spans="1:104 16383:16383">
-      <c r="A4" s="50" t="s">
-        <v>243</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="35"/>
-      <c r="E4" t="s">
-        <v>365</v>
-      </c>
-      <c r="F4" t="s">
-        <v>370</v>
-      </c>
-      <c r="G4" t="s">
-        <v>422</v>
-      </c>
-      <c r="H4" t="s">
-        <v>428</v>
-      </c>
-      <c r="I4" t="s">
-        <v>371</v>
-      </c>
-      <c r="J4" t="s">
-        <v>372</v>
-      </c>
-      <c r="K4" t="s">
-        <v>375</v>
-      </c>
-      <c r="L4" t="s">
-        <v>376</v>
-      </c>
-      <c r="M4" t="s">
-        <v>378</v>
-      </c>
-      <c r="N4" t="s">
-        <v>380</v>
-      </c>
-      <c r="O4" t="s">
-        <v>384</v>
-      </c>
-      <c r="P4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>376</v>
-      </c>
-      <c r="R4" t="s">
-        <v>376</v>
-      </c>
-      <c r="S4" t="s">
-        <v>376</v>
-      </c>
-      <c r="T4" t="s">
-        <v>385</v>
-      </c>
-      <c r="U4" t="s">
-        <v>389</v>
-      </c>
-      <c r="V4" t="s">
-        <v>413</v>
-      </c>
-      <c r="W4" t="s">
-        <v>417</v>
-      </c>
-      <c r="XFC4" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:104 16383:16383">
-      <c r="A5" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>366</v>
       </c>
       <c r="C5" s="30">
         <v>908</v>
@@ -5267,15 +3928,15 @@
         <v>31</v>
       </c>
       <c r="XFC5" t="s">
-        <v>401</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:104 16383:16383">
-      <c r="A6" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>367</v>
+      <c r="A6" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="C6" s="30">
         <v>910</v>
@@ -5283,413 +3944,413 @@
       <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="54"/>
+      <c r="F6" s="44"/>
       <c r="XFC6" t="s">
-        <v>402</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:104 16383:16383">
-      <c r="A7" s="50" t="s">
-        <v>246</v>
+      <c r="A7" s="40" t="s">
+        <v>157</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="6"/>
       <c r="E7" t="s">
-        <v>418</v>
+        <v>329</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
+        <v>330</v>
       </c>
       <c r="G7" t="s">
-        <v>423</v>
+        <v>334</v>
       </c>
       <c r="H7" t="s">
-        <v>429</v>
+        <v>340</v>
       </c>
       <c r="I7" t="s">
-        <v>371</v>
+        <v>282</v>
       </c>
       <c r="J7" t="s">
-        <v>372</v>
+        <v>283</v>
       </c>
       <c r="K7" t="s">
-        <v>375</v>
+        <v>286</v>
       </c>
       <c r="L7" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="M7" t="s">
-        <v>378</v>
+        <v>289</v>
       </c>
       <c r="N7" t="s">
-        <v>380</v>
+        <v>291</v>
       </c>
       <c r="O7" t="s">
-        <v>382</v>
+        <v>293</v>
       </c>
       <c r="P7" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="Q7" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="R7" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="S7" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="T7" t="s">
-        <v>386</v>
+        <v>297</v>
       </c>
       <c r="U7" t="s">
-        <v>387</v>
+        <v>298</v>
       </c>
       <c r="V7" t="s">
-        <v>414</v>
+        <v>325</v>
       </c>
       <c r="W7" t="s">
-        <v>416</v>
+        <v>327</v>
       </c>
       <c r="XFC7" t="s">
-        <v>403</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:104 16383:16383">
-      <c r="A8" s="50" t="s">
-        <v>246</v>
+      <c r="A8" s="40" t="s">
+        <v>157</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="6"/>
       <c r="E8" t="s">
-        <v>434</v>
+        <v>345</v>
       </c>
       <c r="F8" t="s">
-        <v>436</v>
+        <v>347</v>
       </c>
       <c r="G8" t="s">
-        <v>424</v>
+        <v>335</v>
       </c>
       <c r="H8" t="s">
-        <v>430</v>
+        <v>341</v>
       </c>
       <c r="I8" t="s">
-        <v>371</v>
+        <v>282</v>
       </c>
       <c r="J8" t="s">
-        <v>372</v>
+        <v>283</v>
       </c>
       <c r="K8" t="s">
-        <v>432</v>
+        <v>343</v>
       </c>
       <c r="L8" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="M8" t="s">
-        <v>379</v>
+        <v>290</v>
       </c>
       <c r="N8" t="s">
-        <v>381</v>
+        <v>292</v>
       </c>
       <c r="O8" t="s">
-        <v>383</v>
+        <v>294</v>
       </c>
       <c r="P8" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="Q8" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="R8" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="S8" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="T8" t="s">
-        <v>385</v>
+        <v>296</v>
       </c>
       <c r="U8" t="s">
-        <v>388</v>
+        <v>299</v>
       </c>
       <c r="V8" t="s">
-        <v>395</v>
+        <v>306</v>
       </c>
       <c r="W8" t="s">
-        <v>417</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:104 16383:16383">
-      <c r="A9" s="50" t="s">
-        <v>246</v>
+      <c r="A9" s="40" t="s">
+        <v>157</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>435</v>
+        <v>346</v>
       </c>
       <c r="F9" t="s">
-        <v>437</v>
+        <v>348</v>
       </c>
       <c r="G9" t="s">
-        <v>425</v>
+        <v>336</v>
       </c>
       <c r="H9" t="s">
-        <v>431</v>
+        <v>342</v>
       </c>
       <c r="I9" t="s">
-        <v>371</v>
+        <v>282</v>
       </c>
       <c r="J9" t="s">
-        <v>372</v>
+        <v>283</v>
       </c>
       <c r="K9" t="s">
-        <v>433</v>
+        <v>344</v>
       </c>
       <c r="L9" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="M9" t="s">
-        <v>378</v>
+        <v>289</v>
       </c>
       <c r="N9" t="s">
-        <v>380</v>
+        <v>291</v>
       </c>
       <c r="O9" t="s">
-        <v>384</v>
+        <v>295</v>
       </c>
       <c r="P9" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="Q9" t="s">
-        <v>377</v>
+        <v>288</v>
       </c>
       <c r="R9" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="S9" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
       <c r="T9" t="s">
-        <v>386</v>
+        <v>297</v>
       </c>
       <c r="U9" t="s">
-        <v>389</v>
+        <v>300</v>
       </c>
       <c r="V9" t="s">
-        <v>397</v>
+        <v>308</v>
       </c>
       <c r="W9" t="s">
-        <v>415</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:104 16383:16383">
-      <c r="A10" s="50" t="s">
-        <v>247</v>
+      <c r="A10" s="40" t="s">
+        <v>158</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="6"/>
       <c r="XFC10" t="s">
-        <v>404</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:104 16383:16383">
-      <c r="A11" s="50" t="s">
-        <v>248</v>
+      <c r="A11" s="40" t="s">
+        <v>159</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="6"/>
       <c r="XFC11" t="s">
-        <v>405</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:104 16383:16383">
-      <c r="A12" s="50" t="s">
-        <v>249</v>
+      <c r="A12" s="40" t="s">
+        <v>160</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="6"/>
       <c r="XFC12" t="s">
-        <v>406</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:104 16383:16383">
-      <c r="A13" s="50" t="s">
-        <v>250</v>
+      <c r="A13" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="6"/>
       <c r="XFC13" t="s">
-        <v>407</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:104 16383:16383">
-      <c r="A14" s="50" t="s">
-        <v>251</v>
+      <c r="A14" s="40" t="s">
+        <v>162</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>224</v>
+        <v>146</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="6"/>
       <c r="XFC14" t="s">
-        <v>408</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:104 16383:16383">
-      <c r="A15" s="50" t="s">
-        <v>252</v>
+      <c r="A15" s="40" t="s">
+        <v>163</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>225</v>
+        <v>147</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="6"/>
       <c r="XFC15" t="s">
-        <v>409</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:104 16383:16383">
-      <c r="A16" s="50" t="s">
-        <v>253</v>
+      <c r="A16" s="40" t="s">
+        <v>164</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>197</v>
+        <v>138</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="6"/>
       <c r="XFC16" t="s">
-        <v>410</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4 16383:16383">
-      <c r="A17" s="50" t="s">
-        <v>254</v>
+      <c r="A17" s="40" t="s">
+        <v>165</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>198</v>
+        <v>139</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="6"/>
       <c r="XFC17" t="s">
-        <v>391</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4 16383:16383">
-      <c r="A18" s="50" t="s">
-        <v>255</v>
+      <c r="A18" s="40" t="s">
+        <v>166</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>199</v>
+        <v>140</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="6"/>
       <c r="XFC18" t="s">
-        <v>392</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:4 16383:16383">
-      <c r="A19" s="50" t="s">
-        <v>256</v>
+      <c r="A19" s="40" t="s">
+        <v>167</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>200</v>
+        <v>141</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="6"/>
       <c r="XFC19" t="s">
-        <v>393</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:4 16383:16383">
-      <c r="A20" s="50" t="s">
-        <v>257</v>
+      <c r="A20" s="40" t="s">
+        <v>168</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="6"/>
       <c r="XFC20" t="s">
-        <v>394</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:4 16383:16383">
-      <c r="A21" s="50" t="s">
-        <v>258</v>
+      <c r="A21" s="40" t="s">
+        <v>169</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>202</v>
+        <v>143</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="6"/>
       <c r="XFC21" t="s">
-        <v>395</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:4 16383:16383">
-      <c r="A22" s="50" t="s">
-        <v>259</v>
+      <c r="A22" s="40" t="s">
+        <v>170</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>203</v>
+        <v>144</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="6"/>
       <c r="XFC22" t="s">
-        <v>396</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:4 16383:16383">
-      <c r="A23" s="50" t="s">
-        <v>260</v>
+      <c r="A23" s="40" t="s">
+        <v>171</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>204</v>
+        <v>145</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="6"/>
       <c r="XFC23" t="s">
-        <v>390</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:4 16383:16383">
-      <c r="A24" s="52"/>
-      <c r="B24" s="49"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="30"/>
       <c r="D24" s="6"/>
       <c r="XFC24" t="s">
-        <v>397</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:4 16383:16383">
-      <c r="A25" s="52"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="20"/>
       <c r="C25" s="30"/>
       <c r="D25" s="6"/>
       <c r="XFC25" t="s">
-        <v>411</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="1:4 16383:16383">
@@ -5698,7 +4359,7 @@
       <c r="C26" s="30"/>
       <c r="D26" s="6"/>
       <c r="XFC26" t="s">
-        <v>412</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:4 16383:16383">
@@ -5707,7 +4368,7 @@
       <c r="C27" s="30"/>
       <c r="D27" s="6"/>
       <c r="XFC27" t="s">
-        <v>413</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:4 16383:16383">
@@ -5716,7 +4377,7 @@
       <c r="C28" s="30"/>
       <c r="D28" s="6"/>
       <c r="XFC28" t="s">
-        <v>414</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:4 16383:16383">
@@ -5847,366 +4508,350 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="64" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="64" width="29.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="64" width="12.7734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="64" width="10.59375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="64" width="21.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="64" width="23.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="64" width="43.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="64" width="16.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="64" width="23.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="64" width="29.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="64" width="31.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="64" width="32.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="64" width="39.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="64" width="42.85546875" collapsed="true"/>
-    <col min="15" max="16384" style="64" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21" style="54" customWidth="1"/>
+    <col min="2" max="2" width="29" style="54" customWidth="1"/>
+    <col min="3" max="3" width="19" style="54" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="54" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="23" style="54" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" style="54" customWidth="1"/>
+    <col min="8" max="8" width="16" style="54" customWidth="1"/>
+    <col min="9" max="9" width="23" style="54" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" style="54" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="54" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" style="54" customWidth="1"/>
+    <col min="13" max="13" width="39.28515625" style="54" customWidth="1"/>
+    <col min="14" max="14" width="42.85546875" style="54" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="61" t="s">
-        <v>443</v>
-      </c>
-      <c r="F1" s="61" t="s">
-        <v>444</v>
-      </c>
-      <c r="G1" s="61" t="s">
-        <v>445</v>
-      </c>
-      <c r="H1" s="62" t="s">
-        <v>446</v>
-      </c>
-      <c r="I1" s="62" t="s">
-        <v>447</v>
-      </c>
-      <c r="J1" s="62" t="s">
-        <v>448</v>
-      </c>
-      <c r="K1" s="63" t="s">
-        <v>449</v>
-      </c>
-      <c r="L1" s="63" t="s">
-        <v>450</v>
-      </c>
-      <c r="M1" s="63" t="s">
-        <v>451</v>
-      </c>
-      <c r="N1" s="63" t="s">
-        <v>452</v>
+      <c r="E1" s="51" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>355</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>357</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>360</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="M1" s="53" t="s">
+        <v>362</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="38.25" customHeight="1">
-      <c r="A2" s="65" t="s">
-        <v>453</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>454</v>
-      </c>
-      <c r="C2" s="66" t="s">
-        <v>484</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="67">
+      <c r="A2" s="55" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57">
         <v>1111</v>
       </c>
-      <c r="F2" s="67">
+      <c r="F2" s="57">
         <v>111111</v>
       </c>
-      <c r="G2" s="67" t="s">
-        <v>455</v>
-      </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
+      <c r="G2" s="57" t="s">
+        <v>366</v>
+      </c>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="65" t="s">
-        <v>457</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>479</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>485</v>
-      </c>
-      <c r="D3" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="67">
+      <c r="A3" s="55" t="s">
+        <v>368</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57">
         <v>2222</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="57">
         <v>222222</v>
       </c>
-      <c r="G3" s="67" t="s">
-        <v>458</v>
-      </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
+      <c r="G3" s="57" t="s">
+        <v>369</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="65" t="s">
-        <v>459</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>480</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>486</v>
-      </c>
-      <c r="D4" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="67">
+      <c r="A4" s="55" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="57">
         <v>3333</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="57">
         <v>333333</v>
       </c>
-      <c r="G4" s="67" t="s">
-        <v>460</v>
-      </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
+      <c r="G4" s="57" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="65" t="s">
-        <v>461</v>
-      </c>
-      <c r="B5" s="65" t="s">
-        <v>481</v>
-      </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67" t="s">
-        <v>462</v>
-      </c>
-      <c r="I5" s="68" t="s">
-        <v>463</v>
-      </c>
-      <c r="J5" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
+      <c r="A5" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>392</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>374</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="65" t="s">
-        <v>464</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>465</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>487</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="67">
+      <c r="A6" s="55" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>376</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57">
         <v>5555</v>
       </c>
-      <c r="F6" s="67">
+      <c r="F6" s="57">
         <v>555555</v>
       </c>
-      <c r="G6" s="67" t="s">
-        <v>466</v>
-      </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
+      <c r="G6" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="65" t="s">
-        <v>467</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>468</v>
-      </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67">
+      <c r="A7" s="55" t="s">
+        <v>378</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>379</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57">
         <v>6666</v>
       </c>
-      <c r="F7" s="67">
+      <c r="F7" s="57">
         <v>666666</v>
       </c>
-      <c r="G7" s="67" t="s">
-        <v>469</v>
-      </c>
-      <c r="H7" s="67"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
+      <c r="G7" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="H7" s="57"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="65" t="s">
-        <v>470</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>471</v>
-      </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67">
+      <c r="A8" s="55" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>382</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57">
         <v>7777</v>
       </c>
-      <c r="F8" s="67">
+      <c r="F8" s="57">
         <v>777777</v>
       </c>
-      <c r="G8" s="67" t="s">
-        <v>472</v>
-      </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
+      <c r="G8" s="57" t="s">
+        <v>383</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="65" t="s">
-        <v>473</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>474</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67">
+      <c r="A9" s="55" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57">
         <v>8888</v>
       </c>
-      <c r="F9" s="67">
+      <c r="F9" s="57">
         <v>888888</v>
       </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="65" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>476</v>
-      </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67" t="s">
-        <v>462</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>463</v>
-      </c>
-      <c r="J10" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
+      <c r="A10" s="55" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>374</v>
+      </c>
+      <c r="J10" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="65" t="s">
-        <v>477</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>478</v>
-      </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="K11" s="67">
+      <c r="A11" s="55" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>389</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="K11" s="57">
         <v>1111</v>
       </c>
-      <c r="L11" s="67">
+      <c r="L11" s="57">
         <v>3333</v>
       </c>
-      <c r="M11" s="67">
+      <c r="M11" s="57">
         <v>2222</v>
       </c>
-      <c r="N11" s="67">
+      <c r="N11" s="57">
         <v>3333</v>
       </c>
     </row>
@@ -6217,4 +4862,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64" t="s">
+        <v>374</v>
+      </c>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64" t="s">
+        <v>401</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="64" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>404</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64" t="s">
+        <v>374</v>
+      </c>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64" t="s">
+        <v>401</v>
+      </c>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="L3" s="64" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="64" t="s">
+        <v>374</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>394</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>401</v>
+      </c>
+      <c r="H4" s="64">
+        <v>123</v>
+      </c>
+      <c r="I4" s="64" t="s">
+        <v>408</v>
+      </c>
+      <c r="J4" s="64" t="s">
+        <v>288</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="L4" s="64" t="s">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3">
+      <formula1>"A,B,C"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit on 17th sept 2022
</commit_message>
<xml_diff>
--- a/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
+++ b/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AllMastersTestDataInfo" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="418">
   <si>
     <t>Reference ID</t>
   </si>
@@ -1168,57 +1168,24 @@
     <t>AT_UOC_T006</t>
   </si>
   <si>
-    <t>AT_UOC_T006_D6</t>
-  </si>
-  <si>
     <t>Updated Record Approved From Checker</t>
   </si>
   <si>
     <t>AT_UOC_T007_8</t>
   </si>
   <si>
-    <t>AT_UOC_T007__8D7</t>
-  </si>
-  <si>
     <t>Updated Record Rejected From Checker</t>
   </si>
   <si>
     <t>AT_UOC_T009</t>
   </si>
   <si>
-    <t>AT_UOC_T009_D8</t>
-  </si>
-  <si>
-    <t>Updated Record Return to maker</t>
-  </si>
-  <si>
     <t>AT_UOC_T010</t>
   </si>
   <si>
-    <t>AT_UOC_T010_D9</t>
-  </si>
-  <si>
-    <t>AT_UOC_T0011</t>
-  </si>
-  <si>
-    <t>AT_UOC_T0011_D10</t>
-  </si>
-  <si>
     <t>AT_UOC_T0012_13</t>
   </si>
   <si>
-    <t>AT_UOC_T0012__13_D12</t>
-  </si>
-  <si>
-    <t>AT_UOC_T003_D2</t>
-  </si>
-  <si>
-    <t>AT_UOC_T004_D3</t>
-  </si>
-  <si>
-    <t>AT_UOC_T005_D4</t>
-  </si>
-  <si>
     <t>CharecterInputs</t>
   </si>
   <si>
@@ -1265,6 +1232,66 @@
   </si>
   <si>
     <t>Language Id</t>
+  </si>
+  <si>
+    <t>Maker3</t>
+  </si>
+  <si>
+    <t>in02256</t>
+  </si>
+  <si>
+    <t>AT_UOC_T006_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T005_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T004_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T003_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T009_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T010_D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T0012__13_D1</t>
+  </si>
+  <si>
+    <t>Updated Record Return to Maker</t>
+  </si>
+  <si>
+    <t>AT_UOC_T007_8__D1</t>
+  </si>
+  <si>
+    <t>AT_UOC_T011</t>
+  </si>
+  <si>
+    <t>AT_UOC_T011_D1</t>
+  </si>
+  <si>
+    <t>DownloadFilePath</t>
+  </si>
+  <si>
+    <t>C:\\Users\\inindc00076</t>
+  </si>
+  <si>
+    <t>PDFFileName</t>
+  </si>
+  <si>
+    <t>ExcelFileName</t>
+  </si>
+  <si>
+    <t>UnderwriterOffsetControl_export_</t>
+  </si>
+  <si>
+    <t>UnderWriterOffsetControl</t>
+  </si>
+  <si>
+    <t>6706</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1304,7 @@
     <numFmt numFmtId="166" formatCode="[$-409]0"/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1373,8 +1400,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1438,6 +1471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1571,7 +1610,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1711,6 +1750,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -2029,12 +2070,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="11" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="4.140625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" hidden="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="11" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2292,36 +2333,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="21.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="22.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="26" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="24.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="8.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="16384" width="9.140625" style="18" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="31" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="18" width="20.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="18" width="12.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="18" width="7.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="18" width="17.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="18" width="20.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="18" width="20.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="18" width="16.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="18" width="14.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="18" width="16.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="18" width="21.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="18" width="25.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="18" width="21.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="18" width="24.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="18" width="11.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="18" width="22.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="18" width="10.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="18" width="14.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="18" width="26.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="18" width="17.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="18" width="10.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="18" width="16.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="18" width="24.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="18" width="24.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="18" width="8.5703125" collapsed="true"/>
+    <col min="30" max="16384" style="18" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="16" customFormat="1">
@@ -3281,15 +3322,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3327,10 +3368,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>150</v>
+        <v>398</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>399</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>57</v>
@@ -3338,17 +3379,29 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3363,31 +3416,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="43" collapsed="1"/>
-    <col min="13" max="13" width="28" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="76" max="76" width="31.5703125" customWidth="1" collapsed="1"/>
-    <col min="78" max="78" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="89" max="89" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="29" customWidth="1" collapsed="1"/>
-    <col min="98" max="98" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="100" max="100" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="43" width="24.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="73" max="73" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="75" max="75" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="76" max="76" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="78" max="78" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="81" max="81" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="89" max="89" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="93" max="93" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="97" max="97" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="98" max="98" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="100" max="100" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104 16383:16383" s="47" customFormat="1">
@@ -4510,32 +4563,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="54" customWidth="1"/>
-    <col min="2" max="2" width="29" style="54" customWidth="1"/>
-    <col min="3" max="3" width="19" style="54" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="54" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="54" customWidth="1"/>
-    <col min="6" max="6" width="23" style="54" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="54" customWidth="1"/>
-    <col min="8" max="8" width="16" style="54" customWidth="1"/>
-    <col min="9" max="9" width="23" style="54" customWidth="1"/>
-    <col min="10" max="10" width="29.85546875" style="54" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" style="54" customWidth="1"/>
-    <col min="12" max="12" width="32.28515625" style="54" customWidth="1"/>
-    <col min="13" max="13" width="39.28515625" style="54" customWidth="1"/>
-    <col min="14" max="14" width="42.85546875" style="54" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="54"/>
+    <col min="1" max="1" customWidth="true" style="54" width="21.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="54" width="29.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="54" width="12.7734375" collapsed="false" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" style="54" width="19.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="54" width="21.5703125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="54" width="23.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="54" width="43.7109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="54" width="16.0" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="54" width="23.0" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="54" width="29.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="54" width="31.42578125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="54" width="32.28515625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="54" width="39.28515625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="54" width="42.85546875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="54" width="30.28515625" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="54" width="33.28515625" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" style="54" width="35.0" collapsed="false"/>
+    <col min="18" max="16384" style="54" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
+    <row r="1" spans="1:17" ht="15">
       <c r="A1" s="48" t="s">
         <v>61</v>
       </c>
@@ -4578,8 +4634,17 @@
       <c r="N1" s="53" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="38.25" customHeight="1">
+      <c r="O1" s="65" t="s">
+        <v>411</v>
+      </c>
+      <c r="P1" s="65" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q1" s="65" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="38.25" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>364</v>
       </c>
@@ -4606,13 +4671,16 @@
       <c r="L2" s="57"/>
       <c r="M2" s="57"/>
       <c r="N2" s="57"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="57"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="55" t="s">
         <v>368</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -4634,13 +4702,16 @@
       <c r="L3" s="57"/>
       <c r="M3" s="57"/>
       <c r="N3" s="57"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="57"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="55" t="s">
         <v>370</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -4662,13 +4733,16 @@
       <c r="L4" s="57"/>
       <c r="M4" s="57"/>
       <c r="N4" s="57"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="57"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="55" t="s">
         <v>372</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
@@ -4688,13 +4762,16 @@
       <c r="L5" s="57"/>
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="57"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="55" t="s">
         <v>375</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>376</v>
+        <v>400</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="56"/>
@@ -4705,7 +4782,7 @@
         <v>555555</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H6" s="57"/>
       <c r="I6" s="58"/>
@@ -4716,13 +4793,16 @@
       <c r="L6" s="57"/>
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="57"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>379</v>
+        <v>408</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -4733,7 +4813,7 @@
         <v>666666</v>
       </c>
       <c r="G7" s="57" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="58"/>
@@ -4744,13 +4824,16 @@
       <c r="L7" s="57"/>
       <c r="M7" s="57"/>
       <c r="N7" s="57"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="57"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="55" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
@@ -4761,24 +4844,25 @@
         <v>777777</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="58"/>
-      <c r="J8" s="55" t="s">
-        <v>367</v>
-      </c>
+      <c r="J8" s="55"/>
       <c r="K8" s="57"/>
       <c r="L8" s="57"/>
       <c r="M8" s="57"/>
       <c r="N8" s="57"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="57"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="55" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
@@ -4788,7 +4872,9 @@
       <c r="F9" s="57">
         <v>888888</v>
       </c>
-      <c r="G9" s="57"/>
+      <c r="G9" s="57" t="s">
+        <v>407</v>
+      </c>
       <c r="H9" s="57"/>
       <c r="I9" s="58"/>
       <c r="J9" s="55" t="s">
@@ -4798,13 +4884,16 @@
       <c r="L9" s="57"/>
       <c r="M9" s="57"/>
       <c r="N9" s="57"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="57"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="55" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
@@ -4824,15 +4913,20 @@
       <c r="L10" s="57"/>
       <c r="M10" s="57"/>
       <c r="N10" s="57"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="57"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="55" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>389</v>
-      </c>
-      <c r="C11" s="56"/>
+        <v>406</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>417</v>
+      </c>
       <c r="D11" s="56"/>
       <c r="E11" s="57"/>
       <c r="F11" s="57"/>
@@ -4853,6 +4947,15 @@
       </c>
       <c r="N11" s="57">
         <v>3333</v>
+      </c>
+      <c r="O11" s="57" t="s">
+        <v>412</v>
+      </c>
+      <c r="P11" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q11" s="66" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -4868,24 +4971,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="38" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="36.5703125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="17.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="28.7109375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="27.0" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="20.28515625" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="38.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4905,25 +5008,25 @@
         <v>358</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4931,7 +5034,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
@@ -4940,14 +5043,14 @@
       </c>
       <c r="F2" s="64"/>
       <c r="G2" s="64" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="H2" s="64"/>
       <c r="I2" s="64"/>
       <c r="J2" s="64"/>
       <c r="K2" s="3"/>
       <c r="L2" s="64" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4955,7 +5058,7 @@
         <v>130</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
@@ -4964,16 +5067,16 @@
       </c>
       <c r="F3" s="64"/>
       <c r="G3" s="64" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="H3" s="64"/>
       <c r="I3" s="64"/>
       <c r="J3" s="64"/>
       <c r="K3" s="3" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4981,7 +5084,7 @@
         <v>131</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="C4" s="63"/>
       <c r="D4" s="63"/>
@@ -4989,25 +5092,25 @@
         <v>374</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="H4" s="64">
         <v>123</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="J4" s="64" t="s">
         <v>288</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -5025,12 +5128,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 27 feb 2022
</commit_message>
<xml_diff>
--- a/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
+++ b/AzentioULSFramework_Anandh/Test-data/ULSTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="AllMastersTestDataInfo" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="ReportMaster" sheetId="9" r:id="rId9"/>
     <sheet name="ReportMasterTestData_2" sheetId="10" r:id="rId10"/>
     <sheet name="ApplicationDetails_DisbMaker" sheetId="11" r:id="rId11"/>
+    <sheet name="BeneficiaryDetails" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="757">
   <si>
     <t>Master Screen Name</t>
   </si>
@@ -2020,6 +2021,285 @@
   </si>
   <si>
     <t>AT_ADM_002_D1</t>
+  </si>
+  <si>
+    <t>Facility Appliation ID</t>
+  </si>
+  <si>
+    <t>Beneficiary Name</t>
+  </si>
+  <si>
+    <t>Beneficiary Type</t>
+  </si>
+  <si>
+    <t>Beneficiary KYC</t>
+  </si>
+  <si>
+    <t>Beneficiary Address</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>IBAN Account No</t>
+  </si>
+  <si>
+    <t>MICR Type</t>
+  </si>
+  <si>
+    <t>Beneficiary MICR Code</t>
+  </si>
+  <si>
+    <t>Bank Code</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>IFSC Code</t>
+  </si>
+  <si>
+    <t>Payment Type</t>
+  </si>
+  <si>
+    <t>Payment Mode</t>
+  </si>
+  <si>
+    <t>Beneficiary eMail</t>
+  </si>
+  <si>
+    <t>AT-BD-002</t>
+  </si>
+  <si>
+    <t>AT-BD-001</t>
+  </si>
+  <si>
+    <t>AT-BD-003</t>
+  </si>
+  <si>
+    <t>AT-BD-004</t>
+  </si>
+  <si>
+    <t>AT-BD-005</t>
+  </si>
+  <si>
+    <t>AT-BD-006</t>
+  </si>
+  <si>
+    <t>AT-BD-007</t>
+  </si>
+  <si>
+    <t>AT-BD-008</t>
+  </si>
+  <si>
+    <t>AT-BD-009</t>
+  </si>
+  <si>
+    <t>AT-BD-010</t>
+  </si>
+  <si>
+    <t>AT-BD-011</t>
+  </si>
+  <si>
+    <t>AT-BD-012</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D1</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D2</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D3</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D4</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D5</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D6</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D7</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D8</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D9</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D10</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D11</t>
+  </si>
+  <si>
+    <t>AT-BD-001_D12</t>
+  </si>
+  <si>
+    <t>Ready to move / Under construction Property from Builder/Society</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>BT Bank</t>
+  </si>
+  <si>
+    <t>Wall street</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>MICR</t>
+  </si>
+  <si>
+    <t>SBIN001</t>
+  </si>
+  <si>
+    <t>SBI Bank Karnataka</t>
+  </si>
+  <si>
+    <t>SBIN123456</t>
+  </si>
+  <si>
+    <t>On Completion</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>warrentBeffet@gmail.com</t>
+  </si>
+  <si>
+    <t>Durga</t>
+  </si>
+  <si>
+    <t>Prajna</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>Swapnil</t>
+  </si>
+  <si>
+    <t>Mokshan</t>
+  </si>
+  <si>
+    <t>Gowri</t>
+  </si>
+  <si>
+    <t>shwetha</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>Priyanka</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>dalal street</t>
+  </si>
+  <si>
+    <t>Car Steet</t>
+  </si>
+  <si>
+    <t>Mariyamman Kovil Street</t>
+  </si>
+  <si>
+    <t>Lorry street</t>
+  </si>
+  <si>
+    <t>STR Street</t>
+  </si>
+  <si>
+    <t>Sqirrel street</t>
+  </si>
+  <si>
+    <t>Tortoise Street</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Ajith</t>
+  </si>
+  <si>
+    <t>Current Account</t>
+  </si>
+  <si>
+    <t>Card Account</t>
+  </si>
+  <si>
+    <t>FIXED DEPOSIT</t>
+  </si>
+  <si>
+    <t>78965485231</t>
+  </si>
+  <si>
+    <t>54632147802</t>
+  </si>
+  <si>
+    <t>52148796325</t>
+  </si>
+  <si>
+    <t>45132598762</t>
+  </si>
+  <si>
+    <t>12301478965</t>
+  </si>
+  <si>
+    <t>23014587963</t>
+  </si>
+  <si>
+    <t>21450369870</t>
+  </si>
+  <si>
+    <t>52130147863</t>
+  </si>
+  <si>
+    <t>98745103215</t>
+  </si>
+  <si>
+    <t>95215327410</t>
+  </si>
+  <si>
+    <t>12457896305</t>
+  </si>
+  <si>
+    <t>Next Stage Code</t>
+  </si>
+  <si>
+    <t>Disbursment Checker</t>
+  </si>
+  <si>
+    <t>Valid Search</t>
+  </si>
+  <si>
+    <t>InValid Search</t>
+  </si>
+  <si>
+    <t>Tjfsjkdg</t>
+  </si>
+  <si>
+    <t>1586</t>
   </si>
 </sst>
 </file>
@@ -2028,9 +2308,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2151,6 +2431,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2226,7 +2519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2360,11 +2653,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
@@ -2377,8 +2681,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2581,8 +2889,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="10" xfId="11" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="19" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="5"/>
     <cellStyle name="Excel_5f_5f_5f_20_5f_5f_5f_Built-in_5f_5f_5f_20_5f_5f_5f_Normal" xfId="6"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Hyperlink" xfId="7"/>
@@ -2590,6 +2908,7 @@
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="9"/>
     <cellStyle name="Heading" xfId="3"/>
     <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
     <cellStyle name="Hyperlink_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f" xfId="10"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Result" xfId="1"/>
@@ -2897,7 +3216,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2913,14 +3232,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="103.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" style="4" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" style="4" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="103.7109375" style="4"/>
-    <col min="5" max="5" width="31.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33" style="10" customWidth="1"/>
-    <col min="7" max="7" width="6" style="4" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="103.7109375" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="37.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" hidden="true" style="4" width="34.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" hidden="true" style="4" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" style="4" width="103.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="4" width="31.5703125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="10" width="33.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" hidden="true" style="4" width="6.0" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="103.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3116,8 +3435,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="21" width="22" style="70" customWidth="1"/>
-    <col min="22" max="16384" width="11" style="70"/>
+    <col min="1" max="21" customWidth="true" style="70" width="22.0" collapsed="false"/>
+    <col min="22" max="16384" style="70" width="11.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -3360,32 +3679,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" customWidth="1"/>
-    <col min="18" max="18" width="24.42578125" customWidth="1"/>
-    <col min="19" max="19" width="27.85546875" customWidth="1"/>
-    <col min="20" max="20" width="24" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="31.85546875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="12.140625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="30.28515625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="24.28515625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="26.42578125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="18.140625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="14.42578125" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="11.7109375" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="13.85546875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="14.5703125" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="28.140625" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="24.42578125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="27.85546875" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -3511,6 +3830,933 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="11.61328125" collapsed="false" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="68.42578125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="26.7109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="31.7109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="21.7109375" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="30.7109375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="29.42578125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="30.5703125" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="20.28515625" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="18.28515625" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="26.85546875" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="36.140625" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="24.42578125" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="24.5703125" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" width="17.42578125" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" width="18.28515625" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="126" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="126" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1" s="126" t="s">
+        <v>665</v>
+      </c>
+      <c r="G1" s="126" t="s">
+        <v>666</v>
+      </c>
+      <c r="H1" s="126" t="s">
+        <v>667</v>
+      </c>
+      <c r="I1" s="126" t="s">
+        <v>668</v>
+      </c>
+      <c r="J1" s="126" t="s">
+        <v>669</v>
+      </c>
+      <c r="K1" s="126" t="s">
+        <v>670</v>
+      </c>
+      <c r="L1" s="126" t="s">
+        <v>671</v>
+      </c>
+      <c r="M1" s="126" t="s">
+        <v>672</v>
+      </c>
+      <c r="N1" s="126" t="s">
+        <v>673</v>
+      </c>
+      <c r="O1" s="126" t="s">
+        <v>674</v>
+      </c>
+      <c r="P1" s="126" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q1" s="126" t="s">
+        <v>676</v>
+      </c>
+      <c r="R1" s="126" t="s">
+        <v>677</v>
+      </c>
+      <c r="S1" s="126" t="s">
+        <v>678</v>
+      </c>
+      <c r="T1" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="126" t="s">
+        <v>658</v>
+      </c>
+      <c r="V1" s="132" t="s">
+        <v>751</v>
+      </c>
+      <c r="W1" s="132" t="s">
+        <v>753</v>
+      </c>
+      <c r="X1" s="132" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="127" t="s">
+        <v>680</v>
+      </c>
+      <c r="B2" s="127" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F2" s="129" t="s">
+        <v>704</v>
+      </c>
+      <c r="G2" s="129" t="s">
+        <v>705</v>
+      </c>
+      <c r="H2" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="129" t="s">
+        <v>706</v>
+      </c>
+      <c r="J2" s="125" t="s">
+        <v>707</v>
+      </c>
+      <c r="K2" s="124">
+        <v>12345678902</v>
+      </c>
+      <c r="L2" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M2" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N2" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O2" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P2" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q2" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R2" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S2" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T2" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U2" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V2" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="127" t="s">
+        <v>679</v>
+      </c>
+      <c r="B3" s="127" t="s">
+        <v>692</v>
+      </c>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F3" s="129" t="s">
+        <v>715</v>
+      </c>
+      <c r="G3" s="129" t="s">
+        <v>724</v>
+      </c>
+      <c r="H3" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" s="129" t="s">
+        <v>728</v>
+      </c>
+      <c r="J3" s="125" t="s">
+        <v>737</v>
+      </c>
+      <c r="K3" s="129" t="s">
+        <v>740</v>
+      </c>
+      <c r="L3" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M3" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N3" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O3" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P3" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q3" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R3" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S3" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T3" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U3" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V3" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="127" t="s">
+        <v>681</v>
+      </c>
+      <c r="B4" s="127" t="s">
+        <v>693</v>
+      </c>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F4" s="129" t="s">
+        <v>716</v>
+      </c>
+      <c r="G4" s="129" t="s">
+        <v>725</v>
+      </c>
+      <c r="H4" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" s="129" t="s">
+        <v>729</v>
+      </c>
+      <c r="J4" s="125" t="s">
+        <v>738</v>
+      </c>
+      <c r="K4" s="129" t="s">
+        <v>741</v>
+      </c>
+      <c r="L4" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M4" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N4" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O4" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P4" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q4" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R4" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S4" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T4" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U4" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V4" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W4" s="123"/>
+      <c r="X4" s="123"/>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="127" t="s">
+        <v>682</v>
+      </c>
+      <c r="B5" s="127" t="s">
+        <v>694</v>
+      </c>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F5" s="129" t="s">
+        <v>717</v>
+      </c>
+      <c r="G5" s="129" t="s">
+        <v>726</v>
+      </c>
+      <c r="H5" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I5" s="129" t="s">
+        <v>730</v>
+      </c>
+      <c r="J5" s="125" t="s">
+        <v>739</v>
+      </c>
+      <c r="K5" s="129" t="s">
+        <v>742</v>
+      </c>
+      <c r="L5" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M5" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N5" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O5" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P5" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q5" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R5" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S5" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T5" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U5" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V5" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W5" s="123"/>
+      <c r="X5" s="123"/>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="127" t="s">
+        <v>683</v>
+      </c>
+      <c r="B6" s="127" t="s">
+        <v>695</v>
+      </c>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F6" s="129" t="s">
+        <v>718</v>
+      </c>
+      <c r="G6" s="129" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I6" s="129" t="s">
+        <v>731</v>
+      </c>
+      <c r="J6" s="125" t="s">
+        <v>390</v>
+      </c>
+      <c r="K6" s="129" t="s">
+        <v>743</v>
+      </c>
+      <c r="L6" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M6" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N6" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O6" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P6" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q6" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R6" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S6" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T6" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U6" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V6" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="127" t="s">
+        <v>684</v>
+      </c>
+      <c r="B7" s="127" t="s">
+        <v>696</v>
+      </c>
+      <c r="C7" s="128" t="s">
+        <v>756</v>
+      </c>
+      <c r="D7" s="128"/>
+      <c r="E7" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F7" s="129" t="s">
+        <v>719</v>
+      </c>
+      <c r="G7" s="129" t="s">
+        <v>727</v>
+      </c>
+      <c r="H7" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I7" s="129" t="s">
+        <v>732</v>
+      </c>
+      <c r="J7" s="125" t="s">
+        <v>707</v>
+      </c>
+      <c r="K7" s="129" t="s">
+        <v>744</v>
+      </c>
+      <c r="L7" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M7" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N7" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O7" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P7" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q7" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R7" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S7" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T7" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U7" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V7" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="127" t="s">
+        <v>685</v>
+      </c>
+      <c r="B8" s="127" t="s">
+        <v>697</v>
+      </c>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F8" s="129" t="s">
+        <v>735</v>
+      </c>
+      <c r="G8" s="129" t="s">
+        <v>705</v>
+      </c>
+      <c r="H8" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I8" s="129" t="s">
+        <v>733</v>
+      </c>
+      <c r="J8" s="125" t="s">
+        <v>737</v>
+      </c>
+      <c r="K8" s="129" t="s">
+        <v>745</v>
+      </c>
+      <c r="L8" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M8" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N8" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O8" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P8" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q8" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R8" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S8" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T8" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U8" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V8" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="127" t="s">
+        <v>686</v>
+      </c>
+      <c r="B9" s="127" t="s">
+        <v>698</v>
+      </c>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F9" s="129" t="s">
+        <v>736</v>
+      </c>
+      <c r="G9" s="129" t="s">
+        <v>724</v>
+      </c>
+      <c r="H9" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="129" t="s">
+        <v>734</v>
+      </c>
+      <c r="J9" s="125" t="s">
+        <v>738</v>
+      </c>
+      <c r="K9" s="129" t="s">
+        <v>746</v>
+      </c>
+      <c r="L9" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M9" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N9" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O9" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P9" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q9" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R9" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S9" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T9" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U9" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V9" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W9" s="123"/>
+      <c r="X9" s="123"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="127" t="s">
+        <v>687</v>
+      </c>
+      <c r="B10" s="127" t="s">
+        <v>699</v>
+      </c>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F10" s="129" t="s">
+        <v>720</v>
+      </c>
+      <c r="G10" s="129" t="s">
+        <v>725</v>
+      </c>
+      <c r="H10" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I10" s="129" t="s">
+        <v>706</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>739</v>
+      </c>
+      <c r="K10" s="129" t="s">
+        <v>747</v>
+      </c>
+      <c r="L10" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M10" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N10" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O10" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P10" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q10" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R10" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S10" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T10" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U10" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V10" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W10" s="123"/>
+      <c r="X10" s="123"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="127" t="s">
+        <v>688</v>
+      </c>
+      <c r="B11" s="127" t="s">
+        <v>700</v>
+      </c>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F11" s="129" t="s">
+        <v>721</v>
+      </c>
+      <c r="G11" s="129" t="s">
+        <v>726</v>
+      </c>
+      <c r="H11" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I11" s="129" t="s">
+        <v>728</v>
+      </c>
+      <c r="J11" s="125" t="s">
+        <v>390</v>
+      </c>
+      <c r="K11" s="129" t="s">
+        <v>748</v>
+      </c>
+      <c r="L11" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M11" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N11" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O11" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P11" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q11" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R11" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S11" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T11" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U11" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V11" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W11" s="123"/>
+      <c r="X11" s="123"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="127" t="s">
+        <v>689</v>
+      </c>
+      <c r="B12" s="127" t="s">
+        <v>701</v>
+      </c>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F12" s="129" t="s">
+        <v>722</v>
+      </c>
+      <c r="G12" s="129" t="s">
+        <v>390</v>
+      </c>
+      <c r="H12" s="129" t="s">
+        <v>262</v>
+      </c>
+      <c r="I12" s="129" t="s">
+        <v>729</v>
+      </c>
+      <c r="J12" s="125" t="s">
+        <v>707</v>
+      </c>
+      <c r="K12" s="129" t="s">
+        <v>749</v>
+      </c>
+      <c r="L12" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M12" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N12" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O12" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P12" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q12" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R12" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S12" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T12" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U12" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V12" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W12" s="123"/>
+      <c r="X12" s="123"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="127" t="s">
+        <v>690</v>
+      </c>
+      <c r="B13" s="127" t="s">
+        <v>702</v>
+      </c>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="125" t="s">
+        <v>703</v>
+      </c>
+      <c r="F13" s="129" t="s">
+        <v>723</v>
+      </c>
+      <c r="G13" s="129" t="s">
+        <v>727</v>
+      </c>
+      <c r="H13" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="I13" s="129" t="s">
+        <v>730</v>
+      </c>
+      <c r="J13" s="125" t="s">
+        <v>737</v>
+      </c>
+      <c r="K13" s="129" t="s">
+        <v>750</v>
+      </c>
+      <c r="L13" s="125" t="s">
+        <v>708</v>
+      </c>
+      <c r="M13" s="125">
+        <v>44498126</v>
+      </c>
+      <c r="N13" s="129" t="s">
+        <v>709</v>
+      </c>
+      <c r="O13" s="125" t="s">
+        <v>710</v>
+      </c>
+      <c r="P13" s="124" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q13" s="125" t="s">
+        <v>712</v>
+      </c>
+      <c r="R13" s="125" t="s">
+        <v>713</v>
+      </c>
+      <c r="S13" s="130" t="s">
+        <v>714</v>
+      </c>
+      <c r="T13" s="125" t="s">
+        <v>281</v>
+      </c>
+      <c r="U13" s="131" t="s">
+        <v>662</v>
+      </c>
+      <c r="V13" s="131" t="s">
+        <v>752</v>
+      </c>
+      <c r="W13" s="133" t="s">
+        <v>704</v>
+      </c>
+      <c r="X13" s="133" t="s">
+        <v>755</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="S3" r:id="rId2"/>
+    <hyperlink ref="S4" r:id="rId3"/>
+    <hyperlink ref="S5" r:id="rId4"/>
+    <hyperlink ref="S6" r:id="rId5"/>
+    <hyperlink ref="S7" r:id="rId6"/>
+    <hyperlink ref="S8" r:id="rId7"/>
+    <hyperlink ref="S9" r:id="rId8"/>
+    <hyperlink ref="S10" r:id="rId9"/>
+    <hyperlink ref="S11" r:id="rId10"/>
+    <hyperlink ref="S12" r:id="rId11"/>
+    <hyperlink ref="S13" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
@@ -3521,7 +4767,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="62.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="62.5703125" style="4"/>
+    <col min="1" max="16384" style="4" width="62.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3588,36 +4834,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="34" style="28" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="12" style="28" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" style="28" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="34" style="28" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" style="28" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" style="28" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" style="28" customWidth="1"/>
-    <col min="15" max="15" width="35.140625" style="28" customWidth="1"/>
-    <col min="16" max="16" width="41" style="28" customWidth="1"/>
-    <col min="17" max="17" width="35.42578125" style="28" customWidth="1"/>
-    <col min="18" max="18" width="39.5703125" style="28" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" style="28" customWidth="1"/>
-    <col min="20" max="20" width="36.85546875" style="28" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" style="28" customWidth="1"/>
-    <col min="22" max="22" width="23.85546875" style="28" customWidth="1"/>
-    <col min="23" max="23" width="42.5703125" style="28" customWidth="1"/>
-    <col min="24" max="24" width="28.28515625" style="28" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" style="28" customWidth="1"/>
-    <col min="26" max="26" width="26.5703125" style="28" customWidth="1"/>
-    <col min="27" max="27" width="40" style="28" customWidth="1"/>
-    <col min="28" max="28" width="39.5703125" style="28" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" style="28" customWidth="1"/>
-    <col min="30" max="16384" width="15.28515625" style="28"/>
+    <col min="1" max="1" customWidth="true" style="21" width="20.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="21" width="24.5703125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="24" width="20.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="21" width="16.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="21" width="23.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="28" width="34.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="28" width="20.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="28" width="12.0" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="28" width="28.85546875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="28" width="33.28515625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="28" width="34.0" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="28" width="27.28515625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="28" width="23.28515625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="28" width="26.85546875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="28" width="35.140625" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="28" width="41.0" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" style="28" width="35.42578125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="28" width="39.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="28" width="18.85546875" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" style="28" width="36.85546875" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" style="28" width="17.140625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" style="28" width="23.85546875" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" style="28" width="42.5703125" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" style="28" width="28.28515625" collapsed="false"/>
+    <col min="25" max="25" customWidth="true" style="28" width="16.140625" collapsed="false"/>
+    <col min="26" max="26" customWidth="true" style="28" width="26.5703125" collapsed="false"/>
+    <col min="27" max="27" customWidth="true" style="28" width="40.0" collapsed="false"/>
+    <col min="28" max="28" customWidth="true" style="28" width="39.5703125" collapsed="false"/>
+    <col min="29" max="29" customWidth="true" style="28" width="13.28515625" collapsed="false"/>
+    <col min="30" max="16384" style="28" width="15.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1" ht="15">
@@ -4582,10 +5828,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="14.5703125" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="4" width="33.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="4" width="23.85546875" collapsed="false"/>
+    <col min="4" max="16384" style="4" width="14.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4684,117 +5930,117 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="51" style="4" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="46.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="64.28515625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="50.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="51" style="4" customWidth="1"/>
-    <col min="15" max="15" width="37.140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" style="4"/>
-    <col min="18" max="18" width="48.5703125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="42.5703125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="42.140625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="41.28515625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="57.28515625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="39.28515625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="46.140625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="43.28515625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="38.85546875" style="4" customWidth="1"/>
-    <col min="28" max="28" width="41.28515625" style="4" customWidth="1"/>
-    <col min="29" max="29" width="44.28515625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="29.5703125" style="4" customWidth="1"/>
-    <col min="31" max="31" width="37.140625" style="4" customWidth="1"/>
-    <col min="32" max="32" width="41" style="4" customWidth="1"/>
-    <col min="33" max="33" width="46.140625" style="4" customWidth="1"/>
-    <col min="34" max="34" width="42.140625" style="4" customWidth="1"/>
-    <col min="35" max="35" width="34" style="4" customWidth="1"/>
-    <col min="36" max="36" width="43.28515625" style="4" customWidth="1"/>
-    <col min="37" max="37" width="39.85546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="68.140625" style="4" customWidth="1"/>
-    <col min="39" max="39" width="63.42578125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="48.28515625" style="4" customWidth="1"/>
-    <col min="41" max="41" width="35" style="4" customWidth="1"/>
-    <col min="42" max="42" width="50.5703125" style="4" customWidth="1"/>
-    <col min="43" max="43" width="45.7109375" style="4" customWidth="1"/>
-    <col min="44" max="44" width="34" style="4" customWidth="1"/>
-    <col min="45" max="45" width="45.7109375" style="4" customWidth="1"/>
-    <col min="46" max="46" width="14.5703125" style="4"/>
-    <col min="47" max="47" width="36.42578125" style="4" customWidth="1"/>
-    <col min="48" max="48" width="44.7109375" style="4" customWidth="1"/>
-    <col min="49" max="49" width="46" style="4" customWidth="1"/>
-    <col min="50" max="50" width="41" style="4" customWidth="1"/>
-    <col min="51" max="51" width="62.5703125" style="4" customWidth="1"/>
-    <col min="52" max="52" width="53.140625" style="4" customWidth="1"/>
-    <col min="53" max="53" width="55.85546875" style="4" customWidth="1"/>
-    <col min="54" max="54" width="39.28515625" style="4" customWidth="1"/>
-    <col min="55" max="55" width="25.140625" style="4" customWidth="1"/>
-    <col min="56" max="56" width="35.140625" style="4" customWidth="1"/>
-    <col min="57" max="57" width="35.85546875" style="4" customWidth="1"/>
-    <col min="58" max="58" width="34.85546875" style="4" customWidth="1"/>
-    <col min="59" max="59" width="37.140625" style="4" customWidth="1"/>
-    <col min="60" max="60" width="46.7109375" style="4" customWidth="1"/>
-    <col min="61" max="62" width="14.5703125" style="4"/>
-    <col min="63" max="63" width="37.42578125" style="4" customWidth="1"/>
-    <col min="64" max="64" width="49.85546875" style="4" customWidth="1"/>
-    <col min="65" max="65" width="47.28515625" style="4" customWidth="1"/>
-    <col min="66" max="66" width="47.85546875" style="4" customWidth="1"/>
-    <col min="67" max="67" width="59.140625" style="4" customWidth="1"/>
-    <col min="68" max="68" width="45" style="4" customWidth="1"/>
-    <col min="69" max="69" width="35.85546875" style="4" customWidth="1"/>
-    <col min="70" max="70" width="62" style="4" customWidth="1"/>
-    <col min="71" max="71" width="62.7109375" style="4" customWidth="1"/>
-    <col min="72" max="72" width="42.140625" style="4" customWidth="1"/>
-    <col min="73" max="73" width="48.28515625" style="4" customWidth="1"/>
-    <col min="74" max="74" width="47.85546875" style="4" customWidth="1"/>
-    <col min="75" max="75" width="65.28515625" style="4" customWidth="1"/>
-    <col min="76" max="76" width="46.140625" style="4" customWidth="1"/>
-    <col min="77" max="77" width="58.42578125" style="4" customWidth="1"/>
-    <col min="78" max="78" width="54.140625" style="4" customWidth="1"/>
-    <col min="79" max="79" width="46.140625" style="4" customWidth="1"/>
-    <col min="80" max="80" width="50.140625" style="4" customWidth="1"/>
-    <col min="81" max="81" width="53.5703125" style="4" customWidth="1"/>
-    <col min="82" max="82" width="49.5703125" style="4" customWidth="1"/>
-    <col min="83" max="83" width="52.42578125" style="4" customWidth="1"/>
-    <col min="84" max="84" width="66.42578125" style="4" customWidth="1"/>
-    <col min="85" max="85" width="49.42578125" style="4" customWidth="1"/>
-    <col min="86" max="86" width="72.140625" style="4" customWidth="1"/>
-    <col min="87" max="87" width="59.42578125" style="4" customWidth="1"/>
-    <col min="88" max="88" width="51" style="4" customWidth="1"/>
-    <col min="89" max="89" width="39.140625" style="4" customWidth="1"/>
-    <col min="90" max="90" width="45.7109375" style="4" customWidth="1"/>
-    <col min="91" max="91" width="60.85546875" style="4" customWidth="1"/>
-    <col min="92" max="92" width="64.28515625" style="4" customWidth="1"/>
-    <col min="93" max="93" width="57" style="4" customWidth="1"/>
-    <col min="94" max="94" width="73.28515625" style="4" customWidth="1"/>
-    <col min="95" max="95" width="70.7109375" style="4" customWidth="1"/>
-    <col min="96" max="96" width="56.5703125" style="4" customWidth="1"/>
-    <col min="97" max="97" width="44.28515625" style="4" customWidth="1"/>
-    <col min="98" max="98" width="48.7109375" style="4" customWidth="1"/>
-    <col min="99" max="99" width="67" style="4" customWidth="1"/>
-    <col min="100" max="100" width="47.42578125" style="4" customWidth="1"/>
-    <col min="101" max="101" width="42.85546875" style="4" customWidth="1"/>
-    <col min="102" max="102" width="62" style="4" customWidth="1"/>
-    <col min="103" max="103" width="58.5703125" style="4" customWidth="1"/>
-    <col min="104" max="104" width="50" style="4" customWidth="1"/>
-    <col min="105" max="105" width="98.42578125" style="4" customWidth="1"/>
-    <col min="106" max="106" width="58.5703125" style="4" customWidth="1"/>
-    <col min="107" max="107" width="45.28515625" style="4" customWidth="1"/>
-    <col min="108" max="108" width="36.140625" style="4" customWidth="1"/>
-    <col min="109" max="109" width="46.85546875" style="4" customWidth="1"/>
-    <col min="110" max="112" width="56.28515625" style="4" customWidth="1"/>
-    <col min="113" max="113" width="55.85546875" style="4" customWidth="1"/>
-    <col min="114" max="16384" width="14.5703125" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="45.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="4" width="43.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="4" width="34.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="4" width="34.85546875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="4" width="45.7109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="4" width="44.28515625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="4" width="51.0" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="4" width="43.7109375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="4" width="46.7109375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="4" width="64.28515625" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="4" width="50.5703125" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="4" width="46.140625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="4" width="51.0" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="4" width="37.140625" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="4" width="27.28515625" collapsed="false"/>
+    <col min="17" max="17" style="4" width="14.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="4" width="48.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="4" width="42.5703125" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" style="4" width="42.42578125" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" style="4" width="42.140625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" style="4" width="41.28515625" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" style="4" width="57.28515625" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" style="4" width="39.28515625" collapsed="false"/>
+    <col min="25" max="25" customWidth="true" style="4" width="46.140625" collapsed="false"/>
+    <col min="26" max="26" customWidth="true" style="4" width="43.28515625" collapsed="false"/>
+    <col min="27" max="27" customWidth="true" style="4" width="38.85546875" collapsed="false"/>
+    <col min="28" max="28" customWidth="true" style="4" width="41.28515625" collapsed="false"/>
+    <col min="29" max="29" customWidth="true" style="4" width="44.28515625" collapsed="false"/>
+    <col min="30" max="30" customWidth="true" style="4" width="29.5703125" collapsed="false"/>
+    <col min="31" max="31" customWidth="true" style="4" width="37.140625" collapsed="false"/>
+    <col min="32" max="32" customWidth="true" style="4" width="41.0" collapsed="false"/>
+    <col min="33" max="33" customWidth="true" style="4" width="46.140625" collapsed="false"/>
+    <col min="34" max="34" customWidth="true" style="4" width="42.140625" collapsed="false"/>
+    <col min="35" max="35" customWidth="true" style="4" width="34.0" collapsed="false"/>
+    <col min="36" max="36" customWidth="true" style="4" width="43.28515625" collapsed="false"/>
+    <col min="37" max="37" customWidth="true" style="4" width="39.85546875" collapsed="false"/>
+    <col min="38" max="38" customWidth="true" style="4" width="68.140625" collapsed="false"/>
+    <col min="39" max="39" customWidth="true" style="4" width="63.42578125" collapsed="false"/>
+    <col min="40" max="40" customWidth="true" style="4" width="48.28515625" collapsed="false"/>
+    <col min="41" max="41" customWidth="true" style="4" width="35.0" collapsed="false"/>
+    <col min="42" max="42" customWidth="true" style="4" width="50.5703125" collapsed="false"/>
+    <col min="43" max="43" customWidth="true" style="4" width="45.7109375" collapsed="false"/>
+    <col min="44" max="44" customWidth="true" style="4" width="34.0" collapsed="false"/>
+    <col min="45" max="45" customWidth="true" style="4" width="45.7109375" collapsed="false"/>
+    <col min="46" max="46" style="4" width="14.5703125" collapsed="false"/>
+    <col min="47" max="47" customWidth="true" style="4" width="36.42578125" collapsed="false"/>
+    <col min="48" max="48" customWidth="true" style="4" width="44.7109375" collapsed="false"/>
+    <col min="49" max="49" customWidth="true" style="4" width="46.0" collapsed="false"/>
+    <col min="50" max="50" customWidth="true" style="4" width="41.0" collapsed="false"/>
+    <col min="51" max="51" customWidth="true" style="4" width="62.5703125" collapsed="false"/>
+    <col min="52" max="52" customWidth="true" style="4" width="53.140625" collapsed="false"/>
+    <col min="53" max="53" customWidth="true" style="4" width="55.85546875" collapsed="false"/>
+    <col min="54" max="54" customWidth="true" style="4" width="39.28515625" collapsed="false"/>
+    <col min="55" max="55" customWidth="true" style="4" width="25.140625" collapsed="false"/>
+    <col min="56" max="56" customWidth="true" style="4" width="35.140625" collapsed="false"/>
+    <col min="57" max="57" customWidth="true" style="4" width="35.85546875" collapsed="false"/>
+    <col min="58" max="58" customWidth="true" style="4" width="34.85546875" collapsed="false"/>
+    <col min="59" max="59" customWidth="true" style="4" width="37.140625" collapsed="false"/>
+    <col min="60" max="60" customWidth="true" style="4" width="46.7109375" collapsed="false"/>
+    <col min="61" max="62" style="4" width="14.5703125" collapsed="false"/>
+    <col min="63" max="63" customWidth="true" style="4" width="37.42578125" collapsed="false"/>
+    <col min="64" max="64" customWidth="true" style="4" width="49.85546875" collapsed="false"/>
+    <col min="65" max="65" customWidth="true" style="4" width="47.28515625" collapsed="false"/>
+    <col min="66" max="66" customWidth="true" style="4" width="47.85546875" collapsed="false"/>
+    <col min="67" max="67" customWidth="true" style="4" width="59.140625" collapsed="false"/>
+    <col min="68" max="68" customWidth="true" style="4" width="45.0" collapsed="false"/>
+    <col min="69" max="69" customWidth="true" style="4" width="35.85546875" collapsed="false"/>
+    <col min="70" max="70" customWidth="true" style="4" width="62.0" collapsed="false"/>
+    <col min="71" max="71" customWidth="true" style="4" width="62.7109375" collapsed="false"/>
+    <col min="72" max="72" customWidth="true" style="4" width="42.140625" collapsed="false"/>
+    <col min="73" max="73" customWidth="true" style="4" width="48.28515625" collapsed="false"/>
+    <col min="74" max="74" customWidth="true" style="4" width="47.85546875" collapsed="false"/>
+    <col min="75" max="75" customWidth="true" style="4" width="65.28515625" collapsed="false"/>
+    <col min="76" max="76" customWidth="true" style="4" width="46.140625" collapsed="false"/>
+    <col min="77" max="77" customWidth="true" style="4" width="58.42578125" collapsed="false"/>
+    <col min="78" max="78" customWidth="true" style="4" width="54.140625" collapsed="false"/>
+    <col min="79" max="79" customWidth="true" style="4" width="46.140625" collapsed="false"/>
+    <col min="80" max="80" customWidth="true" style="4" width="50.140625" collapsed="false"/>
+    <col min="81" max="81" customWidth="true" style="4" width="53.5703125" collapsed="false"/>
+    <col min="82" max="82" customWidth="true" style="4" width="49.5703125" collapsed="false"/>
+    <col min="83" max="83" customWidth="true" style="4" width="52.42578125" collapsed="false"/>
+    <col min="84" max="84" customWidth="true" style="4" width="66.42578125" collapsed="false"/>
+    <col min="85" max="85" customWidth="true" style="4" width="49.42578125" collapsed="false"/>
+    <col min="86" max="86" customWidth="true" style="4" width="72.140625" collapsed="false"/>
+    <col min="87" max="87" customWidth="true" style="4" width="59.42578125" collapsed="false"/>
+    <col min="88" max="88" customWidth="true" style="4" width="51.0" collapsed="false"/>
+    <col min="89" max="89" customWidth="true" style="4" width="39.140625" collapsed="false"/>
+    <col min="90" max="90" customWidth="true" style="4" width="45.7109375" collapsed="false"/>
+    <col min="91" max="91" customWidth="true" style="4" width="60.85546875" collapsed="false"/>
+    <col min="92" max="92" customWidth="true" style="4" width="64.28515625" collapsed="false"/>
+    <col min="93" max="93" customWidth="true" style="4" width="57.0" collapsed="false"/>
+    <col min="94" max="94" customWidth="true" style="4" width="73.28515625" collapsed="false"/>
+    <col min="95" max="95" customWidth="true" style="4" width="70.7109375" collapsed="false"/>
+    <col min="96" max="96" customWidth="true" style="4" width="56.5703125" collapsed="false"/>
+    <col min="97" max="97" customWidth="true" style="4" width="44.28515625" collapsed="false"/>
+    <col min="98" max="98" customWidth="true" style="4" width="48.7109375" collapsed="false"/>
+    <col min="99" max="99" customWidth="true" style="4" width="67.0" collapsed="false"/>
+    <col min="100" max="100" customWidth="true" style="4" width="47.42578125" collapsed="false"/>
+    <col min="101" max="101" customWidth="true" style="4" width="42.85546875" collapsed="false"/>
+    <col min="102" max="102" customWidth="true" style="4" width="62.0" collapsed="false"/>
+    <col min="103" max="103" customWidth="true" style="4" width="58.5703125" collapsed="false"/>
+    <col min="104" max="104" customWidth="true" style="4" width="50.0" collapsed="false"/>
+    <col min="105" max="105" customWidth="true" style="4" width="98.42578125" collapsed="false"/>
+    <col min="106" max="106" customWidth="true" style="4" width="58.5703125" collapsed="false"/>
+    <col min="107" max="107" customWidth="true" style="4" width="45.28515625" collapsed="false"/>
+    <col min="108" max="108" customWidth="true" style="4" width="36.140625" collapsed="false"/>
+    <col min="109" max="109" customWidth="true" style="4" width="46.85546875" collapsed="false"/>
+    <col min="110" max="112" customWidth="true" style="4" width="56.28515625" collapsed="false"/>
+    <col min="113" max="113" customWidth="true" style="4" width="55.85546875" collapsed="false"/>
+    <col min="114" max="16384" style="4" width="14.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:113" ht="15.75">
@@ -7470,24 +8716,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="16" style="50" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="50" customWidth="1"/>
-    <col min="6" max="7" width="37.7109375" style="50" customWidth="1"/>
-    <col min="8" max="8" width="72.140625" style="50" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" style="50" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" style="50" customWidth="1"/>
-    <col min="11" max="11" width="49.42578125" style="50" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="53.140625" style="50" customWidth="1"/>
-    <col min="14" max="14" width="65.28515625" style="50" customWidth="1"/>
-    <col min="15" max="15" width="70.85546875" style="50" customWidth="1"/>
-    <col min="16" max="16" width="50" style="50" customWidth="1"/>
-    <col min="17" max="17" width="55.28515625" style="50" customWidth="1"/>
-    <col min="18" max="18" width="57.5703125" style="50" customWidth="1"/>
-    <col min="19" max="16384" width="15.28515625" style="50"/>
+    <col min="1" max="1" customWidth="true" style="50" width="34.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="50" width="47.5703125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="50" width="19.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="50" width="16.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="50" width="35.140625" collapsed="false"/>
+    <col min="6" max="7" customWidth="true" style="50" width="37.7109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="50" width="72.140625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="50" width="25.85546875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="50" width="37.7109375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="50" width="49.42578125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="50" width="51.42578125" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="50" width="53.140625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="50" width="65.28515625" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="50" width="70.85546875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="50" width="50.0" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" style="50" width="55.28515625" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="50" width="57.5703125" collapsed="false"/>
+    <col min="19" max="16384" style="50" width="15.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15">
@@ -7937,19 +9183,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="60.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="47.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="44.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="33" style="4" customWidth="1"/>
-    <col min="12" max="12" width="62.7109375" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="14.5703125" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="4" width="32.140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="4" width="25.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="4" width="39.85546875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="4" width="28.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="4" width="60.28515625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="4" width="28.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="4" width="47.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="4" width="44.28515625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="4" width="33.0" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="4" width="62.7109375" collapsed="false"/>
+    <col min="13" max="16384" style="4" width="14.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15">
@@ -8090,41 +9336,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="70" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="70" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="70" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="70" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="70" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="70" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="70" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" style="70" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="70"/>
-    <col min="11" max="11" width="24.140625" style="70" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="70" customWidth="1"/>
-    <col min="13" max="13" width="35.5703125" style="70" customWidth="1"/>
-    <col min="14" max="14" width="17" style="70" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="70" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="70" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" style="70" customWidth="1"/>
-    <col min="18" max="18" width="25.28515625" style="70" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" style="70" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" style="70" customWidth="1"/>
-    <col min="21" max="21" width="25.42578125" style="70" customWidth="1"/>
-    <col min="22" max="22" width="32.85546875" style="70" customWidth="1"/>
-    <col min="23" max="23" width="17.85546875" style="70" customWidth="1"/>
-    <col min="24" max="24" width="30.85546875" style="70" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="70" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" style="70" customWidth="1"/>
-    <col min="27" max="27" width="29.28515625" style="70" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" style="70" customWidth="1"/>
-    <col min="29" max="29" width="26.7109375" style="70" customWidth="1"/>
-    <col min="30" max="30" width="29.5703125" style="70" customWidth="1"/>
-    <col min="31" max="31" width="24.140625" style="70" customWidth="1"/>
-    <col min="32" max="32" width="28.28515625" style="70" customWidth="1"/>
-    <col min="33" max="33" width="25" style="70" customWidth="1"/>
-    <col min="34" max="34" width="11.140625" style="70" customWidth="1"/>
-    <col min="35" max="16384" width="19.140625" style="70"/>
+    <col min="1" max="1" customWidth="true" style="70" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="70" width="25.85546875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="70" width="17.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="70" width="9.5703125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="70" width="22.140625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="70" width="16.28515625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="70" width="21.7109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="70" width="25.42578125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="70" width="28.28515625" collapsed="false"/>
+    <col min="10" max="10" style="70" width="19.140625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="70" width="24.140625" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="70" width="22.42578125" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="70" width="35.5703125" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="70" width="17.0" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="70" width="18.5703125" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="70" width="15.7109375" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" style="70" width="20.28515625" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="70" width="25.28515625" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="70" width="17.5703125" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" style="70" width="16.85546875" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" style="70" width="25.42578125" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" style="70" width="32.85546875" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" style="70" width="17.85546875" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" style="70" width="30.85546875" collapsed="false"/>
+    <col min="25" max="25" customWidth="true" style="70" width="15.85546875" collapsed="false"/>
+    <col min="26" max="26" customWidth="true" style="70" width="21.7109375" collapsed="false"/>
+    <col min="27" max="27" customWidth="true" style="70" width="29.28515625" collapsed="false"/>
+    <col min="28" max="28" customWidth="true" style="70" width="15.7109375" collapsed="false"/>
+    <col min="29" max="29" customWidth="true" style="70" width="26.7109375" collapsed="false"/>
+    <col min="30" max="30" customWidth="true" style="70" width="29.5703125" collapsed="false"/>
+    <col min="31" max="31" customWidth="true" style="70" width="24.140625" collapsed="false"/>
+    <col min="32" max="32" customWidth="true" style="70" width="28.28515625" collapsed="false"/>
+    <col min="33" max="33" customWidth="true" style="70" width="25.0" collapsed="false"/>
+    <col min="34" max="34" customWidth="true" style="70" width="11.140625" collapsed="false"/>
+    <col min="35" max="16384" style="70" width="19.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15">
@@ -8755,12 +10001,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="4"/>
-    <col min="2" max="2" width="46" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="4" customWidth="1"/>
-    <col min="4" max="6" width="13.7109375" style="4"/>
-    <col min="7" max="7" width="38.85546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="13.7109375" style="4"/>
+    <col min="1" max="1" style="4" width="13.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="4" width="46.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="4" width="16.5703125" collapsed="false"/>
+    <col min="4" max="6" style="4" width="13.7109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="4" width="38.85546875" collapsed="false"/>
+    <col min="8" max="16384" style="4" width="13.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30">

</xml_diff>